<commit_message>
Agregada la creacion del arbol del analizador, y correcion de la tabla para el caracter igual
</commit_message>
<xml_diff>
--- a/src/TablaAnalizador.xlsx
+++ b/src/TablaAnalizador.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\ESCOM\Compiladores\Scanner\Scanner\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA172898-67E3-4970-9B28-B17F41C33ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F7D960-CE6D-4A3C-A1F1-05C2DEE869E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4413F436-9050-491D-A568-5FB4766BD033}"/>
   </bookViews>
@@ -384,8 +384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3ACDC8-D293-48FF-91D7-561C24C81E06}">
   <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V23" workbookViewId="0">
-      <selection activeCell="AE44" sqref="AE44"/>
+    <sheetView tabSelected="1" topLeftCell="V16" workbookViewId="0">
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2809,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="V23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W23">
         <v>1</v>
@@ -3023,7 +3023,7 @@
         <v>0</v>
       </c>
       <c r="V25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W25">
         <v>2</v>
@@ -3451,7 +3451,7 @@
         <v>0</v>
       </c>
       <c r="V29">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W29">
         <v>5</v>
@@ -3665,7 +3665,7 @@
         <v>0</v>
       </c>
       <c r="V31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W31">
         <v>3</v>
@@ -3879,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="V33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W33">
         <v>3</v>
@@ -4200,7 +4200,7 @@
         <v>0</v>
       </c>
       <c r="V36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W36">
         <v>2</v>

</xml_diff>